<commit_message>
Updating config and calibration files
</commit_message>
<xml_diff>
--- a/Config/HPVData.xlsx
+++ b/Config/HPVData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15530" windowHeight="7050" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10650" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="HPV" sheetId="6" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="350">
   <si>
     <t>Age</t>
   </si>
@@ -805,9 +805,6 @@
     <t>Probability of Natural Immunity After Infection</t>
   </si>
   <si>
-    <t>hi</t>
-  </si>
-  <si>
     <t>Fonn 2002</t>
   </si>
   <si>
@@ -1063,9 +1060,6 @@
     <t>Dryden-peterson</t>
   </si>
   <si>
-    <t>Montly CC Mortality Rates</t>
-  </si>
-  <si>
     <t>50% of all cervical cancer</t>
   </si>
   <si>
@@ -1079,6 +1073,12 @@
   </si>
   <si>
     <t>Vaccine type (non-16/18)</t>
+  </si>
+  <si>
+    <t>Monthly Undetected CC Mortality Rates</t>
+  </si>
+  <si>
+    <t>Monthy Detected CC Mortality Rates</t>
   </si>
 </sst>
 </file>
@@ -1086,7 +1086,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -1826,7 +1826,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1901,27 +1901,27 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1958,6 +1958,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3419,7 +3427,7 @@
         <v>240</v>
       </c>
       <c r="E20" s="49" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>167</v>
@@ -3897,7 +3905,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:BL85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+    <sheetView topLeftCell="A65" workbookViewId="0">
       <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
@@ -3908,138 +3916,138 @@
   <sheetData>
     <row r="1" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="52" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="2" spans="1:64" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="53" t="s">
+        <v>261</v>
+      </c>
+      <c r="B2" s="54" t="s">
         <v>262</v>
       </c>
-      <c r="B2" s="54" t="s">
+      <c r="C2" s="55" t="s">
         <v>263</v>
       </c>
-      <c r="C2" s="55" t="s">
+      <c r="D2" s="55" t="s">
         <v>264</v>
       </c>
-      <c r="D2" s="55" t="s">
+      <c r="E2" s="55" t="s">
         <v>265</v>
       </c>
-      <c r="E2" s="55" t="s">
+      <c r="F2" s="56" t="s">
         <v>266</v>
       </c>
-      <c r="F2" s="56" t="s">
+      <c r="G2" s="54" t="s">
         <v>267</v>
       </c>
-      <c r="G2" s="54" t="s">
+      <c r="H2" s="55" t="s">
         <v>268</v>
       </c>
-      <c r="H2" s="55" t="s">
+      <c r="I2" s="55" t="s">
         <v>269</v>
       </c>
-      <c r="I2" s="55" t="s">
+      <c r="J2" s="55" t="s">
         <v>270</v>
       </c>
-      <c r="J2" s="55" t="s">
+      <c r="K2" s="56" t="s">
         <v>271</v>
       </c>
-      <c r="K2" s="56" t="s">
+      <c r="L2" s="54" t="s">
         <v>272</v>
       </c>
-      <c r="L2" s="54" t="s">
+      <c r="M2" s="55" t="s">
         <v>273</v>
       </c>
-      <c r="M2" s="55" t="s">
+      <c r="N2" s="55" t="s">
         <v>274</v>
       </c>
-      <c r="N2" s="55" t="s">
+      <c r="O2" s="55" t="s">
         <v>275</v>
       </c>
-      <c r="O2" s="55" t="s">
+      <c r="P2" s="56" t="s">
         <v>276</v>
       </c>
-      <c r="P2" s="56" t="s">
+      <c r="Q2" s="57" t="s">
         <v>277</v>
       </c>
-      <c r="Q2" s="57" t="s">
+      <c r="R2" s="55" t="s">
         <v>278</v>
       </c>
-      <c r="R2" s="55" t="s">
+      <c r="S2" s="55" t="s">
         <v>279</v>
       </c>
-      <c r="S2" s="55" t="s">
+      <c r="T2" s="55" t="s">
         <v>280</v>
       </c>
-      <c r="T2" s="55" t="s">
+      <c r="U2" s="55" t="s">
         <v>281</v>
       </c>
-      <c r="U2" s="55" t="s">
+      <c r="V2" s="56" t="s">
         <v>282</v>
       </c>
-      <c r="V2" s="56" t="s">
+      <c r="W2" s="54" t="s">
         <v>283</v>
       </c>
-      <c r="W2" s="54" t="s">
+      <c r="X2" s="55" t="s">
         <v>284</v>
       </c>
-      <c r="X2" s="55" t="s">
+      <c r="Y2" s="55" t="s">
         <v>285</v>
       </c>
-      <c r="Y2" s="55" t="s">
+      <c r="Z2" s="55" t="s">
         <v>286</v>
       </c>
-      <c r="Z2" s="55" t="s">
+      <c r="AA2" s="56" t="s">
         <v>287</v>
       </c>
-      <c r="AA2" s="56" t="s">
+      <c r="AB2" s="54" t="s">
         <v>288</v>
       </c>
-      <c r="AB2" s="54" t="s">
+      <c r="AC2" s="55" t="s">
         <v>289</v>
       </c>
-      <c r="AC2" s="55" t="s">
+      <c r="AD2" s="55" t="s">
         <v>290</v>
       </c>
-      <c r="AD2" s="55" t="s">
+      <c r="AE2" s="55" t="s">
         <v>291</v>
       </c>
-      <c r="AE2" s="55" t="s">
+      <c r="AF2" s="56" t="s">
         <v>292</v>
       </c>
-      <c r="AF2" s="56" t="s">
+      <c r="AG2" s="54" t="s">
         <v>293</v>
       </c>
-      <c r="AG2" s="54" t="s">
+      <c r="AH2" s="55" t="s">
         <v>294</v>
       </c>
-      <c r="AH2" s="55" t="s">
+      <c r="AI2" s="55" t="s">
         <v>295</v>
       </c>
-      <c r="AI2" s="55" t="s">
+      <c r="AJ2" s="55" t="s">
         <v>296</v>
       </c>
-      <c r="AJ2" s="55" t="s">
+      <c r="AK2" s="56" t="s">
         <v>297</v>
       </c>
-      <c r="AK2" s="56" t="s">
+      <c r="AL2" s="57" t="s">
         <v>298</v>
       </c>
-      <c r="AL2" s="57" t="s">
+      <c r="AM2" s="55" t="s">
         <v>299</v>
       </c>
-      <c r="AM2" s="55" t="s">
+      <c r="AN2" s="55" t="s">
         <v>300</v>
       </c>
-      <c r="AN2" s="55" t="s">
+      <c r="AO2" s="55" t="s">
         <v>301</v>
       </c>
-      <c r="AO2" s="55" t="s">
+      <c r="AP2" s="55" t="s">
         <v>302</v>
       </c>
-      <c r="AP2" s="55" t="s">
+      <c r="AQ2" s="56" t="s">
         <v>303</v>
-      </c>
-      <c r="AQ2" s="56" t="s">
-        <v>304</v>
       </c>
       <c r="AR2" s="54" t="s">
         <v>208</v>
@@ -4107,7 +4115,7 @@
     </row>
     <row r="3" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="50" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B3" s="58">
         <v>0.59145199999999998</v>
@@ -4301,7 +4309,7 @@
     </row>
     <row r="4" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="66" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B4" s="58">
         <v>0.59145199999999998</v>
@@ -4495,7 +4503,7 @@
     </row>
     <row r="5" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="67" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B5" s="58">
         <v>0.59145199999999998</v>
@@ -5077,7 +5085,7 @@
     </row>
     <row r="8" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A8" s="50" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B8" s="68">
         <v>0.43646124999999997</v>
@@ -6823,7 +6831,7 @@
     </row>
     <row r="17" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="73" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B17" s="74">
         <v>0.23293700000000003</v>
@@ -7017,7 +7025,7 @@
     </row>
     <row r="18" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="50" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B18" s="74">
         <v>0.23293700000000003</v>
@@ -7211,12 +7219,12 @@
     </row>
     <row r="21" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A21" s="52" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="22" spans="1:64" x14ac:dyDescent="0.35">
       <c r="B22" s="97" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="23" spans="1:64" x14ac:dyDescent="0.35">
@@ -7228,7 +7236,7 @@
         <v>0.7142857142857143</v>
       </c>
       <c r="D23" s="98" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="24" spans="1:64" x14ac:dyDescent="0.35">
@@ -7240,12 +7248,12 @@
         <v>0.28571428571428575</v>
       </c>
       <c r="D24" s="98" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="25" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A25" s="50" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B25" s="50">
         <f>0</f>
@@ -7254,117 +7262,117 @@
     </row>
     <row r="27" spans="1:64" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="79" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B27" s="80" t="s">
+        <v>312</v>
+      </c>
+      <c r="C27" s="80" t="s">
         <v>313</v>
       </c>
-      <c r="C27" s="80" t="s">
+      <c r="D27" s="80" t="s">
         <v>314</v>
       </c>
-      <c r="D27" s="80" t="s">
+      <c r="E27" s="80" t="s">
         <v>315</v>
       </c>
-      <c r="E27" s="80" t="s">
+      <c r="F27" s="80" t="s">
         <v>316</v>
       </c>
-      <c r="F27" s="80" t="s">
+      <c r="G27" s="80" t="s">
         <v>317</v>
       </c>
-      <c r="G27" s="80" t="s">
+      <c r="H27" s="80" t="s">
         <v>318</v>
       </c>
-      <c r="H27" s="80" t="s">
+      <c r="I27" s="80" t="s">
         <v>319</v>
       </c>
-      <c r="I27" s="80" t="s">
+      <c r="J27" s="80" t="s">
         <v>320</v>
       </c>
-      <c r="J27" s="80" t="s">
-        <v>321</v>
-      </c>
       <c r="K27" s="80" t="s">
+        <v>322</v>
+      </c>
+      <c r="L27" s="80" t="s">
         <v>323</v>
       </c>
-      <c r="L27" s="80" t="s">
+      <c r="M27" s="80" t="s">
         <v>324</v>
       </c>
-      <c r="M27" s="80" t="s">
+      <c r="N27" s="80" t="s">
         <v>325</v>
       </c>
-      <c r="N27" s="80" t="s">
+      <c r="O27" s="80" t="s">
         <v>326</v>
       </c>
-      <c r="O27" s="80" t="s">
+      <c r="P27" s="80" t="s">
+        <v>329</v>
+      </c>
+      <c r="Q27" s="80" t="s">
         <v>327</v>
       </c>
-      <c r="P27" s="80" t="s">
-        <v>330</v>
-      </c>
-      <c r="Q27" s="80" t="s">
+      <c r="R27" s="80" t="s">
         <v>328</v>
       </c>
-      <c r="R27" s="80" t="s">
+      <c r="V27" s="79" t="s">
+        <v>261</v>
+      </c>
+      <c r="W27" s="80" t="s">
+        <v>312</v>
+      </c>
+      <c r="X27" s="80" t="s">
+        <v>313</v>
+      </c>
+      <c r="Y27" s="80" t="s">
+        <v>314</v>
+      </c>
+      <c r="Z27" s="80" t="s">
+        <v>315</v>
+      </c>
+      <c r="AA27" s="80" t="s">
+        <v>316</v>
+      </c>
+      <c r="AB27" s="80" t="s">
+        <v>317</v>
+      </c>
+      <c r="AC27" s="80" t="s">
+        <v>318</v>
+      </c>
+      <c r="AD27" s="80" t="s">
+        <v>319</v>
+      </c>
+      <c r="AE27" s="80" t="s">
+        <v>320</v>
+      </c>
+      <c r="AF27" s="80" t="s">
+        <v>322</v>
+      </c>
+      <c r="AG27" s="80" t="s">
+        <v>323</v>
+      </c>
+      <c r="AH27" s="80" t="s">
+        <v>324</v>
+      </c>
+      <c r="AI27" s="80" t="s">
+        <v>325</v>
+      </c>
+      <c r="AJ27" s="80" t="s">
+        <v>326</v>
+      </c>
+      <c r="AK27" s="80" t="s">
         <v>329</v>
       </c>
-      <c r="V27" s="79" t="s">
-        <v>262</v>
-      </c>
-      <c r="W27" s="80" t="s">
-        <v>313</v>
-      </c>
-      <c r="X27" s="80" t="s">
-        <v>314</v>
-      </c>
-      <c r="Y27" s="80" t="s">
-        <v>315</v>
-      </c>
-      <c r="Z27" s="80" t="s">
-        <v>316</v>
-      </c>
-      <c r="AA27" s="80" t="s">
-        <v>317</v>
-      </c>
-      <c r="AB27" s="80" t="s">
-        <v>318</v>
-      </c>
-      <c r="AC27" s="80" t="s">
-        <v>319</v>
-      </c>
-      <c r="AD27" s="80" t="s">
-        <v>320</v>
-      </c>
-      <c r="AE27" s="80" t="s">
-        <v>321</v>
-      </c>
-      <c r="AF27" s="80" t="s">
-        <v>323</v>
-      </c>
-      <c r="AG27" s="80" t="s">
-        <v>324</v>
-      </c>
-      <c r="AH27" s="80" t="s">
-        <v>325</v>
-      </c>
-      <c r="AI27" s="80" t="s">
-        <v>326</v>
-      </c>
-      <c r="AJ27" s="80" t="s">
+      <c r="AL27" s="80" t="s">
         <v>327</v>
       </c>
-      <c r="AK27" s="80" t="s">
-        <v>330</v>
-      </c>
-      <c r="AL27" s="80" t="s">
+      <c r="AM27" s="80" t="s">
         <v>328</v>
-      </c>
-      <c r="AM27" s="80" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="28" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="50" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B28" s="50">
         <f t="array" ref="B28:B43">B23*B3:B18+B24*W3:W18+B25*AR3:AR18</f>
@@ -7435,7 +7443,7 @@
         <v>1.3352380952380953E-3</v>
       </c>
       <c r="V28" s="50" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="W28" s="58">
         <v>0.78637999999999997</v>
@@ -7494,7 +7502,7 @@
     </row>
     <row r="29" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="66" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B29" s="50">
         <v>0.59184142857142863</v>
@@ -7548,7 +7556,7 @@
         <v>1.3352380952380953E-3</v>
       </c>
       <c r="V29" s="66" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="W29" s="58">
         <v>0.78637999999999997</v>
@@ -7604,7 +7612,7 @@
     </row>
     <row r="30" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="67" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B30" s="50">
         <v>0.59184142857142863</v>
@@ -7658,7 +7666,7 @@
         <v>1.3352380952380953E-3</v>
       </c>
       <c r="V30" s="67" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="W30" s="58">
         <v>0.78637999999999997</v>
@@ -7934,7 +7942,7 @@
     </row>
     <row r="33" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A33" s="50" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B33" s="50">
         <v>0.43680510714285714</v>
@@ -7988,7 +7996,7 @@
         <v>1.4111071428571429E-2</v>
       </c>
       <c r="V33" s="50" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="W33" s="68">
         <v>0.62775775</v>
@@ -8924,7 +8932,7 @@
     </row>
     <row r="42" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="73" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B42" s="50">
         <v>0.23315357142857146</v>
@@ -8978,7 +8986,7 @@
         <v>3.8157761904761903E-2</v>
       </c>
       <c r="V42" s="73" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="W42" s="74">
         <v>0.36699399999999999</v>
@@ -9034,7 +9042,7 @@
     </row>
     <row r="43" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="50" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B43" s="50">
         <v>0.23315357142857146</v>
@@ -9088,7 +9096,7 @@
         <v>3.8157761904761903E-2</v>
       </c>
       <c r="V43" s="50" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="W43" s="74">
         <v>0.36699399999999999</v>
@@ -9144,101 +9152,101 @@
     </row>
     <row r="45" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A45" s="50" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="L45" s="50" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="V45" s="50" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="46" spans="1:39" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A46" s="79" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B46" s="80" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C46" s="80" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D46" s="80" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E46" s="80" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F46" s="80" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G46" s="80" t="s">
+        <v>317</v>
+      </c>
+      <c r="H46" s="80" t="s">
+        <v>323</v>
+      </c>
+      <c r="I46" s="80" t="s">
+        <v>327</v>
+      </c>
+      <c r="L46" s="79" t="s">
+        <v>261</v>
+      </c>
+      <c r="M46" s="80" t="s">
+        <v>313</v>
+      </c>
+      <c r="N46" s="80" t="s">
         <v>318</v>
       </c>
-      <c r="H46" s="80" t="s">
+      <c r="O46" s="80" t="s">
         <v>324</v>
       </c>
-      <c r="I46" s="80" t="s">
+      <c r="P46" s="80" t="s">
         <v>328</v>
       </c>
-      <c r="L46" s="79" t="s">
-        <v>262</v>
-      </c>
-      <c r="M46" s="80" t="s">
-        <v>314</v>
-      </c>
-      <c r="N46" s="80" t="s">
-        <v>319</v>
-      </c>
-      <c r="O46" s="80" t="s">
-        <v>325</v>
-      </c>
-      <c r="P46" s="80" t="s">
-        <v>329</v>
-      </c>
       <c r="Q46" s="80" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="R46" s="80" t="s">
+        <v>317</v>
+      </c>
+      <c r="S46" s="80" t="s">
+        <v>323</v>
+      </c>
+      <c r="T46" s="80" t="s">
+        <v>327</v>
+      </c>
+      <c r="V46" s="79" t="s">
+        <v>261</v>
+      </c>
+      <c r="W46" s="80" t="s">
+        <v>313</v>
+      </c>
+      <c r="X46" s="80" t="s">
         <v>318</v>
       </c>
-      <c r="S46" s="80" t="s">
+      <c r="Y46" s="80" t="s">
         <v>324</v>
       </c>
-      <c r="T46" s="80" t="s">
+      <c r="Z46" s="80" t="s">
         <v>328</v>
       </c>
-      <c r="V46" s="79" t="s">
-        <v>262</v>
-      </c>
-      <c r="W46" s="80" t="s">
-        <v>314</v>
-      </c>
-      <c r="X46" s="80" t="s">
-        <v>319</v>
-      </c>
-      <c r="Y46" s="80" t="s">
-        <v>325</v>
-      </c>
-      <c r="Z46" s="80" t="s">
-        <v>329</v>
-      </c>
       <c r="AA46" s="80" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="AB46" s="80" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AC46" s="80" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AD46" s="80" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="47" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A47" s="50" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B47" s="51">
         <f t="array" ref="B47:B62">((C28:C43+D28:D43) +C28:C43)/2</f>
@@ -9272,7 +9280,7 @@
         <v>7.1309142857142863E-2</v>
       </c>
       <c r="L47" s="50" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="M47" s="51">
         <f t="array" ref="M47:M62">((X28:X43+Y28:Y43) +X28:X43)/2</f>
@@ -9307,7 +9315,7 @@
         <v>0.12066450000000001</v>
       </c>
       <c r="V47" s="50" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="W47" s="51">
         <f t="array" ref="W47:W62">0.8*M47:M62</f>
@@ -9344,7 +9352,7 @@
     </row>
     <row r="48" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A48" s="66" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B48" s="51">
         <v>0.24213857142857145</v>
@@ -9371,7 +9379,7 @@
         <v>7.1309142857142863E-2</v>
       </c>
       <c r="L48" s="66" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="M48" s="51">
         <v>0.14676349999999999</v>
@@ -9398,7 +9406,7 @@
         <v>0.12066450000000001</v>
       </c>
       <c r="V48" s="66" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="W48" s="51">
         <v>0.1174108</v>
@@ -9427,7 +9435,7 @@
     </row>
     <row r="49" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A49" s="67" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B49" s="51">
         <v>0.24213857142857145</v>
@@ -9454,7 +9462,7 @@
         <v>7.1309142857142863E-2</v>
       </c>
       <c r="L49" s="67" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="M49" s="51">
         <v>0.14676349999999999</v>
@@ -9481,7 +9489,7 @@
         <v>0.12066450000000001</v>
       </c>
       <c r="V49" s="67" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="W49" s="51">
         <v>0.1174108</v>
@@ -9676,7 +9684,7 @@
     </row>
     <row r="52" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A52" s="50" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B52" s="51">
         <v>0.12906128571428571</v>
@@ -9703,7 +9711,7 @@
         <v>5.3409928571428567E-2</v>
       </c>
       <c r="L52" s="50" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="M52" s="51">
         <v>7.678299999999999E-2</v>
@@ -9730,7 +9738,7 @@
         <v>9.0632875000000002E-2</v>
       </c>
       <c r="V52" s="50" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="W52" s="51">
         <v>6.1426399999999992E-2</v>
@@ -10423,7 +10431,7 @@
     </row>
     <row r="61" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A61" s="73" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B61" s="51">
         <v>9.6256928571428563E-2</v>
@@ -10450,7 +10458,7 @@
         <v>9.9361666666666678E-3</v>
       </c>
       <c r="L61" s="73" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="M61" s="51">
         <v>5.6984E-2</v>
@@ -10477,7 +10485,7 @@
         <v>1.7070999999999999E-2</v>
       </c>
       <c r="V61" s="73" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="W61" s="51">
         <v>4.5587200000000001E-2</v>
@@ -10506,7 +10514,7 @@
     </row>
     <row r="62" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A62" s="50" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B62" s="51">
         <v>9.6256928571428563E-2</v>
@@ -10533,7 +10541,7 @@
         <v>9.9361666666666678E-3</v>
       </c>
       <c r="L62" s="50" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="M62" s="51">
         <v>5.6984E-2</v>
@@ -10560,7 +10568,7 @@
         <v>1.7070999999999999E-2</v>
       </c>
       <c r="V62" s="50" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="W62" s="51">
         <v>4.5587200000000001E-2</v>
@@ -11209,7 +11217,7 @@
       </c>
       <c r="W16" s="4"/>
       <c r="Y16" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="Z16" s="48">
         <v>0.09</v>
@@ -11232,7 +11240,7 @@
         <v>0.81</v>
       </c>
       <c r="Z17" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="18" spans="19:27" x14ac:dyDescent="0.35">
@@ -11337,8 +11345,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:U30"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11367,7 +11375,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
@@ -11392,8 +11400,8 @@
       <c r="J2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="26">
-        <v>1.7399999999999999E-2</v>
+      <c r="K2" s="103">
+        <v>3.8999999999999998E-3</v>
       </c>
       <c r="N2" s="12" t="s">
         <v>73</v>
@@ -11414,7 +11422,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -11440,8 +11448,8 @@
       <c r="J3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="K3" s="26">
-        <v>7.3499999999999996E-2</v>
+      <c r="K3" s="104">
+        <v>0.1333</v>
       </c>
       <c r="N3" s="4" t="s">
         <v>74</v>
@@ -11462,7 +11470,7 @@
         <v>21.7</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="5" t="s">
         <v>25</v>
       </c>
@@ -11482,7 +11490,7 @@
       <c r="J4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="K4" s="26">
+      <c r="K4" s="104">
         <v>0.17460000000000001</v>
       </c>
       <c r="N4" s="4" t="s">
@@ -11691,7 +11699,7 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C13" s="40">
         <f>AVERAGE(C3:C5)</f>
@@ -11709,123 +11717,186 @@
     <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+        <v>348</v>
+      </c>
+      <c r="F22" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
+        <v>331</v>
+      </c>
+      <c r="C23" t="s">
         <v>332</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>333</v>
       </c>
-      <c r="D23" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="F23" s="105" t="s">
+        <v>331</v>
+      </c>
+      <c r="G23" s="105" t="s">
+        <v>332</v>
+      </c>
+      <c r="H23" s="105" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
+        <v>338</v>
+      </c>
+      <c r="B24" s="40">
+        <v>1.8098080000000002E-2</v>
+      </c>
+      <c r="C24" s="40">
+        <v>2.3311134000000001E-2</v>
+      </c>
+      <c r="D24" s="40">
+        <v>0.10089910600000002</v>
+      </c>
+      <c r="F24" s="106">
+        <v>1.6014704604402373E-2</v>
+      </c>
+      <c r="G24" s="106">
+        <v>1.9269924863845597E-2</v>
+      </c>
+      <c r="H24" s="106">
+        <v>6.6828048101634521E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>339</v>
       </c>
-      <c r="B24" s="40">
-        <v>8.0070000000000002E-3</v>
-      </c>
-      <c r="C24" s="40">
-        <v>1.9269999999999999E-2</v>
-      </c>
-      <c r="D24" s="40">
-        <v>6.6827999999999999E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+      <c r="B25" s="40">
+        <v>2.1976240000000001E-2</v>
+      </c>
+      <c r="C25" s="40">
+        <v>2.8306377000000004E-2</v>
+      </c>
+      <c r="D25" s="40">
+        <v>0.10089910600000002</v>
+      </c>
+      <c r="F25" s="106">
+        <v>1.9446427019631455E-2</v>
+      </c>
+      <c r="G25" s="106">
+        <v>2.3399194477526798E-2</v>
+      </c>
+      <c r="H25" s="106">
+        <v>6.6828048101634521E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>340</v>
       </c>
-      <c r="B25" s="40">
-        <v>9.7230000000000007E-3</v>
-      </c>
-      <c r="C25" s="40">
-        <v>2.3399E-2</v>
-      </c>
-      <c r="D25" s="40">
-        <v>8.1147999999999998E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+      <c r="B26" s="40">
+        <v>2.6677040000000003E-2</v>
+      </c>
+      <c r="C26" s="40">
+        <v>3.4361216999999999E-2</v>
+      </c>
+      <c r="D26" s="40">
+        <v>0.10089910600000002</v>
+      </c>
+      <c r="F26" s="106">
+        <v>2.3606090553242462E-2</v>
+      </c>
+      <c r="G26" s="106">
+        <v>2.8404369766837342E-2</v>
+      </c>
+      <c r="H26" s="106">
+        <v>6.6828048101634521E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>341</v>
       </c>
-      <c r="B26" s="40">
-        <v>1.1802999999999999E-2</v>
-      </c>
-      <c r="C26" s="40">
-        <v>2.8403999999999999E-2</v>
-      </c>
-      <c r="D26" s="40">
-        <v>9.8505999999999996E-2</v>
-      </c>
-      <c r="N26" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>342</v>
-      </c>
       <c r="B27" s="40">
-        <v>1.4298999999999999E-2</v>
+        <v>3.2318E-2</v>
       </c>
       <c r="C27" s="40">
-        <v>3.4410999999999997E-2</v>
+        <v>4.1627024999999998E-2</v>
       </c>
       <c r="D27" s="40">
-        <v>0.119336</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+        <v>0.10089910600000002</v>
+      </c>
+      <c r="F27" s="106">
+        <v>2.8597686793575668E-2</v>
+      </c>
+      <c r="G27" s="106">
+        <v>3.4410580114009999E-2</v>
+      </c>
+      <c r="H27" s="106">
+        <v>6.6828048101634521E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B28" s="40">
-        <v>8.0070000000000002E-3</v>
+        <v>1.8098080000000002E-2</v>
       </c>
       <c r="C28" s="40">
-        <v>1.9269999999999999E-2</v>
+        <v>2.3311134000000001E-2</v>
       </c>
       <c r="D28" s="40">
-        <v>6.6827999999999999E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+        <v>0.10089910600000002</v>
+      </c>
+      <c r="F28" s="106">
+        <v>1.6014704604402373E-2</v>
+      </c>
+      <c r="G28" s="106">
+        <v>1.9269924863845597E-2</v>
+      </c>
+      <c r="H28" s="106">
+        <v>6.6828048101634521E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>64</v>
       </c>
       <c r="B29" s="40">
-        <v>5.1999999999999998E-3</v>
+        <v>5.8760000000000001E-3</v>
       </c>
       <c r="C29" s="40">
-        <v>1.2513E-2</v>
+        <v>1.5137100000000001E-2</v>
       </c>
       <c r="D29" s="40">
-        <v>4.3395000000000003E-2</v>
+        <v>6.5518900000000005E-2</v>
       </c>
       <c r="E29" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+        <v>342</v>
+      </c>
+      <c r="F29" s="106">
+        <v>5.1995794170137579E-3</v>
+      </c>
+      <c r="G29" s="106">
+        <v>1.2512938223276362E-2</v>
+      </c>
+      <c r="H29" s="106">
+        <v>4.3394836429632801E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E30" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding comments to explain code
</commit_message>
<xml_diff>
--- a/Config/HPVData.xlsx
+++ b/Config/HPVData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\HHCoM\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\CISNET\HHCoM\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10650" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="HPV" sheetId="6" r:id="rId1"/>
@@ -1189,7 +1189,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC5D9F1"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1826,7 +1826,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1953,9 +1953,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1966,6 +1963,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2796,8 +2797,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T47"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36:M38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R21" sqref="R21:R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3218,7 +3219,7 @@
       <c r="Q12" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="R12" s="101">
+      <c r="R12" s="100">
         <f>1/R3</f>
         <v>1</v>
       </c>
@@ -3259,15 +3260,15 @@
       <c r="Q13" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="R13" s="101">
+      <c r="R13" s="100">
         <f>1/R4</f>
         <v>0.32051282051282048</v>
       </c>
-      <c r="S13" s="101">
+      <c r="S13" s="100">
         <f t="shared" ref="S13:T15" si="0">1/S4</f>
         <v>0.42372881355932207</v>
       </c>
-      <c r="T13" s="101">
+      <c r="T13" s="100">
         <f t="shared" si="0"/>
         <v>0.24271844660194175</v>
       </c>
@@ -3302,15 +3303,15 @@
       <c r="Q14" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="R14" s="101">
+      <c r="R14" s="100">
         <f>1/R5</f>
         <v>0.17301038062283736</v>
       </c>
-      <c r="S14" s="101">
+      <c r="S14" s="100">
         <f t="shared" si="0"/>
         <v>0.23980815347721823</v>
       </c>
-      <c r="T14" s="101">
+      <c r="T14" s="100">
         <f t="shared" si="0"/>
         <v>0.12376237623762376</v>
       </c>
@@ -3334,15 +3335,15 @@
       <c r="Q15" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="R15" s="101">
+      <c r="R15" s="100">
         <f>1/R6</f>
         <v>9.8716683119447174E-2</v>
       </c>
-      <c r="S15" s="101">
+      <c r="S15" s="100">
         <f t="shared" si="0"/>
         <v>0.13661202185792348</v>
       </c>
-      <c r="T15" s="101">
+      <c r="T15" s="100">
         <f t="shared" si="0"/>
         <v>7.1225071225071226E-2</v>
       </c>
@@ -3449,23 +3450,23 @@
       <c r="A21" s="45" t="s">
         <v>198</v>
       </c>
-      <c r="B21" s="100">
+      <c r="B21" s="107">
         <v>2</v>
       </c>
-      <c r="C21" s="100">
+      <c r="C21" s="107">
         <v>3</v>
       </c>
-      <c r="D21" s="100">
+      <c r="D21" s="107">
         <v>3.2</v>
       </c>
-      <c r="E21" s="40">
+      <c r="E21" s="106">
         <f t="array" ref="E21:E24">0.7*B21:B24+0.2*C21:C24 +0.1*D21:D24</f>
         <v>2.3200000000000003</v>
       </c>
       <c r="Q21" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="R21" s="11">
+      <c r="R21" s="26">
         <v>1</v>
       </c>
       <c r="S21" s="11">
@@ -3479,16 +3480,16 @@
       <c r="A22" s="45" t="s">
         <v>199</v>
       </c>
-      <c r="B22" s="100">
+      <c r="B22" s="107">
         <v>1.8</v>
       </c>
-      <c r="C22" s="100">
+      <c r="C22" s="107">
         <v>2.8</v>
       </c>
-      <c r="D22" s="100">
+      <c r="D22" s="107">
         <v>3</v>
       </c>
-      <c r="E22" s="40">
+      <c r="E22" s="106">
         <v>2.12</v>
       </c>
       <c r="G22" s="24" t="s">
@@ -3497,7 +3498,7 @@
       <c r="Q22" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="R22" s="11">
+      <c r="R22" s="26">
         <v>2.2000000000000002</v>
       </c>
       <c r="S22" s="11">
@@ -3511,16 +3512,16 @@
       <c r="A23" s="45" t="s">
         <v>241</v>
       </c>
-      <c r="B23" s="100">
+      <c r="B23" s="107">
         <v>1.7</v>
       </c>
-      <c r="C23" s="100">
+      <c r="C23" s="107">
         <v>2.6</v>
       </c>
-      <c r="D23" s="100">
+      <c r="D23" s="107">
         <v>2.8</v>
       </c>
-      <c r="E23" s="40">
+      <c r="E23" s="106">
         <v>1.99</v>
       </c>
       <c r="G23" s="13" t="s">
@@ -3534,7 +3535,7 @@
       <c r="Q23" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="R23" s="11">
+      <c r="R23" s="26">
         <v>5.5</v>
       </c>
       <c r="S23" s="11">
@@ -3548,16 +3549,16 @@
       <c r="A24" s="47" t="s">
         <v>201</v>
       </c>
-      <c r="B24" s="100">
+      <c r="B24" s="107">
         <v>1.5</v>
       </c>
-      <c r="C24" s="100">
+      <c r="C24" s="107">
         <v>2.4</v>
       </c>
-      <c r="D24" s="100">
+      <c r="D24" s="107">
         <v>2.5</v>
       </c>
-      <c r="E24" s="40">
+      <c r="E24" s="106">
         <v>1.7799999999999998</v>
       </c>
       <c r="G24" s="4" t="s">
@@ -3572,9 +3573,9 @@
       <c r="Q24" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="R24" s="102"/>
-      <c r="S24" s="102"/>
-      <c r="T24" s="102"/>
+      <c r="R24" s="101"/>
+      <c r="S24" s="101"/>
+      <c r="T24" s="101"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.35">
       <c r="G25" s="9" t="s">
@@ -3905,8 +3906,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:BL85"/>
   <sheetViews>
-    <sheetView topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView topLeftCell="U22" workbookViewId="0">
+      <selection activeCell="I81" sqref="I81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10756,7 +10757,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AF26"/>
   <sheetViews>
-    <sheetView topLeftCell="S10" workbookViewId="0">
+    <sheetView topLeftCell="U1" workbookViewId="0">
       <selection activeCell="AD23" sqref="AD23"/>
     </sheetView>
   </sheetViews>
@@ -11345,8 +11346,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:U30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O3" sqref="O3:Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11400,7 +11401,7 @@
       <c r="J2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="103">
+      <c r="K2" s="102">
         <v>3.8999999999999998E-3</v>
       </c>
       <c r="N2" s="12" t="s">
@@ -11426,7 +11427,7 @@
       <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="26">
         <f>1</f>
         <v>1</v>
       </c>
@@ -11448,19 +11449,19 @@
       <c r="J3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="K3" s="104">
+      <c r="K3" s="103">
         <v>0.1333</v>
       </c>
       <c r="N3" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="O3" s="4">
+      <c r="O3" s="26">
         <v>4.03</v>
       </c>
-      <c r="P3" s="4">
+      <c r="P3" s="26">
         <v>1.46</v>
       </c>
-      <c r="Q3" s="4">
+      <c r="Q3" s="26">
         <v>11.1</v>
       </c>
       <c r="T3" s="19" t="s">
@@ -11474,7 +11475,7 @@
       <c r="A4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="26">
         <f>3-2</f>
         <v>1</v>
       </c>
@@ -11490,19 +11491,19 @@
       <c r="J4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="K4" s="104">
+      <c r="K4" s="103">
         <v>0.17460000000000001</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="O4" s="4">
+      <c r="O4" s="26">
         <v>2.44</v>
       </c>
-      <c r="P4" s="4">
+      <c r="P4" s="26">
         <v>1.3</v>
       </c>
-      <c r="Q4" s="4">
+      <c r="Q4" s="26">
         <v>4.55</v>
       </c>
       <c r="T4" s="20" t="s">
@@ -11516,7 +11517,7 @@
       <c r="A5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="26">
         <f>20-4</f>
         <v>16</v>
       </c>
@@ -11532,13 +11533,13 @@
       <c r="N5" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="O5" s="4">
+      <c r="O5" s="26">
         <v>1.47</v>
       </c>
-      <c r="P5" s="4">
+      <c r="P5" s="26">
         <v>0.95</v>
       </c>
-      <c r="Q5" s="4">
+      <c r="Q5" s="26">
         <v>2.29</v>
       </c>
       <c r="T5" s="3" t="s">
@@ -11549,7 +11550,7 @@
       <c r="A6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="26">
         <f t="shared" ref="B6:B11" si="0">20-4</f>
         <v>16</v>
       </c>
@@ -11565,13 +11566,13 @@
       <c r="N6" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="O6" s="4">
+      <c r="O6" s="26">
         <v>0.89</v>
       </c>
-      <c r="P6" s="4">
+      <c r="P6" s="26">
         <v>0.46</v>
       </c>
-      <c r="Q6" s="4">
+      <c r="Q6" s="26">
         <v>1.72</v>
       </c>
     </row>
@@ -11579,7 +11580,7 @@
       <c r="A7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="26">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
@@ -11600,7 +11601,7 @@
       <c r="A8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="26">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
@@ -11627,7 +11628,7 @@
       <c r="A9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="26">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
@@ -11655,7 +11656,7 @@
       <c r="A10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="26">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
@@ -11680,7 +11681,7 @@
       <c r="A11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="26">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
@@ -11743,13 +11744,13 @@
       <c r="D23" t="s">
         <v>333</v>
       </c>
-      <c r="F23" s="105" t="s">
+      <c r="F23" s="104" t="s">
         <v>331</v>
       </c>
-      <c r="G23" s="105" t="s">
+      <c r="G23" s="104" t="s">
         <v>332</v>
       </c>
-      <c r="H23" s="105" t="s">
+      <c r="H23" s="104" t="s">
         <v>333</v>
       </c>
     </row>
@@ -11766,13 +11767,13 @@
       <c r="D24" s="40">
         <v>0.10089910600000002</v>
       </c>
-      <c r="F24" s="106">
+      <c r="F24" s="105">
         <v>1.6014704604402373E-2</v>
       </c>
-      <c r="G24" s="106">
+      <c r="G24" s="105">
         <v>1.9269924863845597E-2</v>
       </c>
-      <c r="H24" s="106">
+      <c r="H24" s="105">
         <v>6.6828048101634521E-2</v>
       </c>
     </row>
@@ -11789,13 +11790,13 @@
       <c r="D25" s="40">
         <v>0.10089910600000002</v>
       </c>
-      <c r="F25" s="106">
+      <c r="F25" s="105">
         <v>1.9446427019631455E-2</v>
       </c>
-      <c r="G25" s="106">
+      <c r="G25" s="105">
         <v>2.3399194477526798E-2</v>
       </c>
-      <c r="H25" s="106">
+      <c r="H25" s="105">
         <v>6.6828048101634521E-2</v>
       </c>
     </row>
@@ -11812,13 +11813,13 @@
       <c r="D26" s="40">
         <v>0.10089910600000002</v>
       </c>
-      <c r="F26" s="106">
+      <c r="F26" s="105">
         <v>2.3606090553242462E-2</v>
       </c>
-      <c r="G26" s="106">
+      <c r="G26" s="105">
         <v>2.8404369766837342E-2</v>
       </c>
-      <c r="H26" s="106">
+      <c r="H26" s="105">
         <v>6.6828048101634521E-2</v>
       </c>
     </row>
@@ -11835,13 +11836,13 @@
       <c r="D27" s="40">
         <v>0.10089910600000002</v>
       </c>
-      <c r="F27" s="106">
+      <c r="F27" s="105">
         <v>2.8597686793575668E-2</v>
       </c>
-      <c r="G27" s="106">
+      <c r="G27" s="105">
         <v>3.4410580114009999E-2</v>
       </c>
-      <c r="H27" s="106">
+      <c r="H27" s="105">
         <v>6.6828048101634521E-2</v>
       </c>
     </row>
@@ -11858,13 +11859,13 @@
       <c r="D28" s="40">
         <v>0.10089910600000002</v>
       </c>
-      <c r="F28" s="106">
+      <c r="F28" s="105">
         <v>1.6014704604402373E-2</v>
       </c>
-      <c r="G28" s="106">
+      <c r="G28" s="105">
         <v>1.9269924863845597E-2</v>
       </c>
-      <c r="H28" s="106">
+      <c r="H28" s="105">
         <v>6.6828048101634521E-2</v>
       </c>
     </row>
@@ -11884,13 +11885,13 @@
       <c r="E29" t="s">
         <v>342</v>
       </c>
-      <c r="F29" s="106">
+      <c r="F29" s="105">
         <v>5.1995794170137579E-3</v>
       </c>
-      <c r="G29" s="106">
+      <c r="G29" s="105">
         <v>1.2512938223276362E-2</v>
       </c>
-      <c r="H29" s="106">
+      <c r="H29" s="105">
         <v>4.3394836429632801E-2</v>
       </c>
     </row>
@@ -11910,7 +11911,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:AC64"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>

</xml_diff>